<commit_message>
Fix text capitalization in sp_description.py
</commit_message>
<xml_diff>
--- a/input_data/data_errors_2/4_descricao/descricao.xlsx
+++ b/input_data/data_errors_2/4_descricao/descricao.xlsx
@@ -55,7 +55,7 @@
     <t xml:space="preserve">meta</t>
   </si>
   <si>
-    <t xml:space="preserve">Exemplo com 
+    <t xml:space="preserve">Exemplo com
  CR meio</t>
   </si>
   <si>
@@ -74,7 +74,7 @@
     <t xml:space="preserve">6.2,6.3,6.4</t>
   </si>
   <si>
-    <t xml:space="preserve">Exemplo com 
+    <t xml:space="preserve">Exemplo com
  LF meio</t>
   </si>
   <si>
@@ -414,21 +414,21 @@
   </sheetPr>
   <dimension ref="A1:Y866"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="D1" activeCellId="0" sqref="D1"/>
-      <selection pane="bottomLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.85"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="27.87"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="126.15"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="102.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="126.14"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="102.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="7.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="2" width="24.57"/>

</xml_diff>

<commit_message>
close #87: Check for vertical bar character in all data files
</commit_message>
<xml_diff>
--- a/input_data/data_errors_2/4_descricao/descricao.xlsx
+++ b/input_data/data_errors_2/4_descricao/descricao.xlsx
@@ -151,7 +151,7 @@
     <t xml:space="preserve">4.2,6.1</t>
   </si>
   <si>
-    <t xml:space="preserve">Capacidade adaptativa</t>
+    <t xml:space="preserve">Capacidade | adaptativa</t>
   </si>
   <si>
     <t xml:space="preserve">Índice de capacidade adaptativa</t>
@@ -163,7 +163,7 @@
     <t xml:space="preserve">Capacidade do sistema socioecológico de se preparar e se ajustar às alterações climáticas ou aos danos climáticos potenciais relacionados à seca, principalmente para diminuir os impactos negativos, aproveitar as oportunidades ou responder às consequências. O Índice de Capacidade Adaptativa é resultante da composição dos indicadores temáticos: logística da produção e abastecimento, planejamento e gestão da segurança alimentar e nutricional, manutenção da produção agropecuária, e capacidade socioeconômica familiar.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;ADGER, W. N. Vulnerability. Global Environmental Change, v. 16, n. 3, p. 268–281, ago. 2006.&lt;br&gt;GALLOPÍN, G. C.. Box 1: A systemic synthesis of the relations between vulnerability, hazard, exposure and impact, aimed at policy identification. In: Economic Commission for Latin American and the Caribbean (ECLAC). Handbook for Estimating the Socio-Economic and Environmental Effects of Disasters. Mexico, D.F.: ECLAC, LC/MEX/G.S., p. 2-5, 2003.&lt;br&gt;GALLOPÍN, G. C.. Linkages between vulnerability, resilience, and adaptive capacity. Global Environmental Change, v. 16, p. 293-303, 2006.&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp.</t>
   </si>
   <si>
-    <t xml:space="preserve">Produção e comercialização</t>
+    <t xml:space="preserve">Produção e come|rcialização</t>
   </si>
   <si>
     <t xml:space="preserve">Produção e comercialização de alimentos</t>
@@ -415,12 +415,12 @@
   <dimension ref="A1:Y866"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="bottomLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.55078125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.42"/>

</xml_diff>

<commit_message>
Update test case to check for 10 errors instead of 2
</commit_message>
<xml_diff>
--- a/input_data/data_errors_2/4_descricao/descricao.xlsx
+++ b/input_data/data_errors_2/4_descricao/descricao.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="55">
   <si>
     <t xml:space="preserve">codigo</t>
   </si>
@@ -154,13 +154,159 @@
     <t xml:space="preserve">Capacidade | adaptativa</t>
   </si>
   <si>
-    <t xml:space="preserve">Índice de capacidade adaptativa</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Índice de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">capacidade adaptativa</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Capacidade do sistema socioecológico de se ajustar a possíveis ameaças climáticas de seca.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Capacidade do sistema </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">| </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">socioecológico de se ajustar a possíveis ameaças climáticas de seca.</t>
+    </r>
   </si>
   <si>
-    <t xml:space="preserve">Capacidade do sistema socioecológico de se preparar e se ajustar às alterações climáticas ou aos danos climáticos potenciais relacionados à seca, principalmente para diminuir os impactos negativos, aproveitar as oportunidades ou responder às consequências. O Índice de Capacidade Adaptativa é resultante da composição dos indicadores temáticos: logística da produção e abastecimento, planejamento e gestão da segurança alimentar e nutricional, manutenção da produção agropecuária, e capacidade socioeconômica familiar.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;ADGER, W. N. Vulnerability. Global Environmental Change, v. 16, n. 3, p. 268–281, ago. 2006.&lt;br&gt;GALLOPÍN, G. C.. Box 1: A systemic synthesis of the relations between vulnerability, hazard, exposure and impact, aimed at policy identification. In: Economic Commission for Latin American and the Caribbean (ECLAC). Handbook for Estimating the Socio-Economic and Environmental Effects of Disasters. Mexico, D.F.: ECLAC, LC/MEX/G.S., p. 2-5, 2003.&lt;br&gt;GALLOPÍN, G. C.. Linkages between vulnerability, resilience, and adaptive capacity. Global Environmental Change, v. 16, p. 293-303, 2006.&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp.</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">Capacidade do sistema socioecológico de </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> se preparar e se ajustar às alterações climáticas ou aos danos climáticos potenciais relacionados à seca, principalmente para diminuir os impactos negativos, aproveitar as oportunidades ou responder às consequências. O Índice de Capacidade Adaptativa é resultante da composição dos indicadores temáticos: logística da produção e abastecimento, planejamento e gestão da segurança alimentar e nutricional, manutenção da produção agropecuária, e capacidade socioeconômica familiar.&lt;br&gt;&lt;br&gt;Fontes:&lt;br&gt;ADGER, W. N. Vulnerability. Global Environmental Change, v. 16, n. 3, p. 268–281, ago. 2006.&lt;br&gt;GALLOPÍN, G. C.. Box 1: A systemic synthesis of the relations between vulnerability, hazard, exposure and impact, aimed at policy identification. In: Economic Commission for Latin American and the Caribbean (ECLAC). Handbook for Estimating the Socio-Economic and Environmental Effects of Disasters. Mexico, D.F.: ECLAC, LC/MEX/G.S., p. 2-5, 2003.&lt;br&gt;GALLOPÍN, G. C.. Linkages between vulnerability, resilience, and adaptive capacity. Global Environmental Change, v. 16, p. 293-303, 2006.&lt;br&gt;INTERGOVERNMENTAL PANEL ON CLIMATE CHANGE - IPCC. Climate Change 2014: Synthesis Report. Working Groups I, II and III to the Fifth Assessment Report of the Intergovernmental Panel on Climate Change [Core Writing Team, R.K. Pachauri and L.A. Meyer (eds.)]. IPCC, Geneva, Switzerland, 151 pp.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">AdaptaBrasil </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">MCTI/INPE</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">4.2,</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">|</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">6.1</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">Produção e come|rcialização</t>
@@ -195,7 +341,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="#,##0"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -225,6 +371,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -415,18 +567,18 @@
   <dimension ref="A1:Y866"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A7" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="bottomLeft" activeCell="F7" activeCellId="0" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.5625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.5703125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="9.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="6.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="2" width="51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="27.87"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="5.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="2" width="15.84"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="2" width="126.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="2" width="102.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="21.57"/>
@@ -795,10 +947,10 @@
         <v>-1</v>
       </c>
       <c r="J8" s="5" t="s">
-        <v>15</v>
+        <v>45</v>
       </c>
       <c r="K8" s="5" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="L8" s="5"/>
       <c r="M8" s="5"/>
@@ -823,17 +975,17 @@
         <v>5</v>
       </c>
       <c r="C9" s="9" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="D9" s="9" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="E9" s="9"/>
       <c r="F9" s="5" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="G9" s="5" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="H9" s="8" t="n">
         <v>0</v>
@@ -870,17 +1022,17 @@
         <v>5</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="E10" s="9"/>
       <c r="F10" s="5" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="G10" s="5" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="H10" s="8" t="n">
         <v>0</v>

</xml_diff>